<commit_message>
Install MAST & Polished Building System
Added MAST grid tool plus polishment of prior BuildingManager script. Created also CheckBuildPlaceMgr and disabled all wall limits as they were conflicting with placement of buildings. Rescale building prefabs and created building Placeholder prefabs (just in case).
</commit_message>
<xml_diff>
--- a/Assets/Inventory/Babylon - Asset_Inventory_Template.xlsx
+++ b/Assets/Inventory/Babylon - Asset_Inventory_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mas_c\OneDrive\Escritorio\Unity Projects Desktop\Babylon Rising\Babylon\Assets\Inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7BF731-2126-4367-9DA5-5513BF470F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA3324D-C3B9-4B2E-84BC-CD2511D327FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{01B14A2B-A28C-7B4F-8941-09249883C81A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>Asset Group</t>
   </si>
@@ -152,13 +152,37 @@
   </si>
   <si>
     <t>ok to use and modify</t>
+  </si>
+  <si>
+    <t>Editor Rich Presence</t>
+  </si>
+  <si>
+    <t>https://assetstore.unity.com/packages/tools/level-design/mast-modular-asset-staging-tool-154939</t>
+  </si>
+  <si>
+    <t>MAST is an editor extension for Unity, primarily intended for staging 3D modular assets. It is very useful for making scenes and levels that are based off of a grid. Instead of having to drag a prefab into the inspector, then manually move, rotate and flip it, MAST provides a simple interface that lets you do all the above before ever placing the item in your scene.</t>
+  </si>
+  <si>
+    <t>MAST - Modular Asset Staging Tool</t>
+  </si>
+  <si>
+    <t>Creator</t>
+  </si>
+  <si>
+    <t>Fertile Soils Productions</t>
+  </si>
+  <si>
+    <t>Tools</t>
+  </si>
+  <si>
+    <t>Level-Design</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -218,6 +242,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -236,10 +268,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -255,8 +288,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -572,7 +607,7 @@
   <dimension ref="A2:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -604,8 +639,20 @@
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="H3" s="5" t="s">
         <v>5</v>
       </c>
@@ -613,8 +660,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E4" s="3"/>
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="H4" s="7" t="s">
         <v>6</v>
       </c>
@@ -684,6 +748,9 @@
     <row r="34" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="35" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{48FE5082-C516-4471-AB76-F95079EFF179}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>